<commit_message>
Tackling OTP for US Foods Bot
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/ordering/OrderFiles/Ithaca Bakery/combined_orders.xlsx
+++ b/WorkBot/main/backend/ordering/OrderFiles/Ithaca Bakery/combined_orders.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,44 +429,34 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Triphammer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Downtown</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Easthill</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Downtown</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Collegetown</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Triphammer</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Smoked Salmon (Sliced)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Monin - Guava Puree</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -478,156 +468,126 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Goat Cheese</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Monin - Coconut</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kilogram Chai Concentrate</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+          <t>Mop Head Cut (White)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>3</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hazelnut Coffee (Grounded, Bulk)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Container - Soup (32oz)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Torani - White Chocolate Sauce</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Hot Sauce - Tabasco</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Torani - Caramel Sauce</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>4</t>
+          <t>Chili Sauce - Sriracha</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Torani - Dark Chocolate Sauce</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
+          <t>Peanut Butter - Creamy</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Container - Deli (16oz)</t>
+          <t>Wrap Foil - 9x10.75</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Lid - Deli (6/32oz)</t>
+          <t>Wrap Paper - 15x10.75</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -637,17 +597,22 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Register Tape - Thermal (3.125" x 230')</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+          <t>Cup - Portion (3.25oz)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -659,26 +624,36 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Container - Plastic Clamshell (6")</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Lid - Portion (3.25oz)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Scrubbies - Steel</t>
+          <t>Wrap Paper - 6x10.75</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -695,75 +670,70 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Monin - Guava Puree</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>12</t>
+          <t>Register Tape - Thermal (3.125" x 230')</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mop Head Cut (White)</t>
+          <t>Tea Bags - Earl Grey Lavender (Twinings)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jam - Strawberry</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Tea Bags - Decaf English Breakfast (Twinings)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Wrap Foil - 9x10.75</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Tea Bags - Lemon Ginger (Twinings)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Wrap Paper - 15x10.75</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Monin - Vanilla Sugar Free</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -771,106 +741,126 @@
           <t>1</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Tea Bags - Irish Breakfast (Twinings)</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
+          <t>Monin - Hazelnut</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Tea Bags - Earl Grey (Twinings)</t>
+          <t>Monin - Toffee Nut</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Tea Bags - Darjeeling (Twinings)</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Monin - Lavender</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Tea Bags - Lemon Ginger (Twinings)</t>
+          <t>Monin - Cookie Butter</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Tea Bags - Pomegrantate &amp; Rasp (Twinings)</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Box Cake - 8x8x5</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Monin - Orange</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Degreaser - for Panini Press (Dawn)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -882,7 +872,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Monin - Cranberry</t>
+          <t>Matcha - Jade Leaf</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -892,144 +882,134 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Monin - Caramel Sugar Free</t>
+          <t>Torani - Caramel Sauce</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Monin - Vanilla Sugar Free</t>
+          <t>Torani - White Chocolate Sauce</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Monin - Hazelnut</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Torani - Dark Chocolate Sauce</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Monin - Toffee Nut</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Lid Espresso - 4oz</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Monin - Lavender</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Cup - Hot (8oz)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Monin - Cookie Butter</t>
+          <t>Lid - Hot Cup (8oz)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Box Cake - 8x8x5</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
+          <t>Flax Seeds</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1038,12 +1018,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Degreaser - for Panini Press (Dawn)</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>PKT Salt</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1055,92 +1030,107 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Matcha - Jade Leaf</t>
+          <t>Smoked Salmon (Sliced)</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Grandma's Coffee Cake - Cinnamon w/ Nuts</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Goat Cheese</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Grandma's Coffee Cake - Chocolate Chip</t>
+          <t>Kilogram Chai Concentrate</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Grandma's Coffee Cake - Lemon Poppy</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Container - Deli (16oz)</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Grandma's Coffee Cake - Banana Walnut</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Lid - Deli (6/32oz)</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Joe Tea - Black Unsweetened</t>
+          <t>Java Box (160oz)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1152,12 +1142,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Joe Tea - Ginsens Green</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Container - Plastic Clamshell (6")</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1169,12 +1159,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Joe Tea - Half &amp; Half</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>FRZ Fruit - Mango</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1191,7 +1176,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Joe Tea - Mango Lemonade</t>
+          <t>FRZ Fruit - Raspberry (Whole)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1201,14 +1186,19 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Celsius - Vibe Peach, Tropical, Arctic</t>
+          <t>FRZ Fruit - Blueberry</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1216,24 +1206,24 @@
           <t>1</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="D43" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Bragg - Honey &amp; Green Tea</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
+          <t>Grandma's Coffee Cake - Apple</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1242,10 +1232,10 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bragg - Ginger Lemon Honey</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
+          <t>Grandma's Coffee Cake - Blueberry</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1254,10 +1244,10 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Bragg - Apple Cinn</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
+          <t>Saratoga Sparkling 28oz</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1266,24 +1256,24 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Cup - Portion (3.25oz)</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Joe Tea - Black Cherry</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Lid - Portion (3.25oz)</t>
+          <t>Joe Tea - Black Unsweetened</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1291,24 +1281,29 @@
           <t>1</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Tamper Evident - 12oz Bowl (Smoothie)</t>
+          <t>Joe Tea - Half &amp; Half</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1317,34 +1312,64 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Wrap Paper - 6x10.75</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Joe Tea - Lemon</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Chili Sauce - Sriracha</t>
+          <t>Joe Tea - Peach</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Iced Tea - Raspberry</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
+          <t>Celsius - Vibe Peach, Tropical, Arctic</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1353,44 +1378,39 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Iced Tea - Green Citrus Ginko</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Celsius - Orange, Kiwi Guava</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Chobani - Drinkable Yogurt</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Tea Bags - English Breakfast (Twinings)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>FRZ Fruit - Raspberry (Whole)</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
+          <t>Monin - White Chocolate</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -1399,7 +1419,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Tea Bags - Earl Grey Lavender (Twinings)</t>
+          <t>Honey - Jug</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1411,41 +1431,41 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Tea Bags - English Breakfast (Twinings)</t>
+          <t>Evian 1L</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>4</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Peanut Butter - Creamy</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Container - Soup (16oz)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Monin - White Chocolate</t>
+          <t>Peanut Butter - Chunky</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1457,73 +1477,73 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Honey - Jug</t>
+          <t>Monin - Toasted Marshmallow</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Evian 1L</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Lid - Soup (6/16 oz)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Cup - Hot (8oz)</t>
+          <t>Fiji Water 1L</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Container - Soup (16oz)</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>5</t>
+          <t>Essentia Water</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Peanut Butter - Chunky</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Capers</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1532,7 +1552,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Monin - Toasted Marshmallow</t>
+          <t>Urnex - Cafiza</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1544,20 +1564,15 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Monin - Butter Pecan</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Red Bull</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1566,7 +1581,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Lid - Soup (6/16 oz)</t>
+          <t>Non-Dairy Creamer</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1578,12 +1593,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Fiji Water 1L</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Monin - Orange</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1595,15 +1605,20 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Capers</t>
+          <t>Hazelnut Coffee (Grounded, Bulk)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1612,7 +1627,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Urnex - Rinza</t>
+          <t>Chobani - Drinkable Yogurt</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1624,12 +1644,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Red Bull</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Cup - Portion (2oz)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1637,16 +1652,16 @@
           <t>2</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Lid Espresso - 4oz</t>
+          <t>Vita Coco - Coconut Water 1L</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1658,32 +1673,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Fiji Water 500ml</t>
+          <t>Joe Tea - Ginsens Green</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Cup - Espresso (4oz)</t>
+          <t>Supplement - Collagen</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1692,58 +1702,43 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Celsius - Orange, Kiwi Guava</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Red Bull - Yellow</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Cup - Portion (2oz)</t>
+          <t>Plate - Paper (7")</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Joe Tea - Peach</t>
+          <t>Monin - Caramel Sugar Free</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Red Bull - Watermelon Red</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Joe Tea - Kiwi Strawberry</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1755,7 +1750,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Red Bull - Berry</t>
+          <t>Ithaca Soda - Ginger Beer</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1763,7 +1758,7 @@
           <t>1</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1772,12 +1767,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Red Bull - Amber</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>Container - Deli (8oz)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1785,7 +1775,7 @@
           <t>1</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1794,19 +1784,29 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Panini Sheets - 16x8 3/8</t>
+          <t>Bag Paper - Baguette</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Joe Tea - Classic Lemonade</t>
+          <t>Whitefish Salad</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1818,7 +1818,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Cup Carrier - Fiber (4-Cup)</t>
+          <t>Scrubbies - Steel</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -1830,168 +1830,163 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Whitefish Salad</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>Lid - Portion (2oz)</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Firehook - Everything Bagel</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>4</t>
+          <t>Container - Soup (8oz)</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Firehook - Garlic Thyme</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>4</t>
+          <t>Cup - Espresso (4oz)</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Firehook - Multigrain Flax</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>4</t>
+          <t>Fiji Water 500ml</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Nat's Nuts - Vanilla Rum Cashews</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Saratoga Sparkling 12oz</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Nat's Nuts - Sweet Cayenne Peanuts</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Ithaca Soda - Root Beer</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Nat's Nuts - Cinnamon Whiskey Pecans</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>3</t>
+          <t>Joe Tea - Mango Lemonade</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>DV - Banana Chips</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>12</t>
+          <t>Monin - Blueberry</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>DV - Chocolate Mini Pretzel</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>12</t>
+          <t>Monin - Butter Pecan</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>DV - Sour Neon Gummi Worms</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>6</t>
+          <t>DV - Gummi Peach Rings</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Lid - Portion (2oz)</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>DV - Ginger Slices</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Bag Paper - Baguette</t>
+          <t>Smoked Salmon (Retail Pack)</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Container - Soup (8oz)</t>
+          <t>Hot Chocolate (Bulk)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Essentia Water</t>
+          <t>Lid - Soup (32oz)</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2003,7 +1998,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Ithaca Soda - Ginger Beer</t>
+          <t>Tissues/Kleenex</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2015,7 +2010,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Ithaca Soda - Root Beer</t>
+          <t>Urnex - Brewer Cleaner</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2027,7 +2022,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Lid - Hot Cup (8oz)</t>
+          <t>Red Bull - Berry</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2039,294 +2034,22 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Monin - Blueberry</t>
+          <t>Grandma's Coffee Cake - Cinnamon</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Red Bull - Yellow</t>
+          <t>Sweet Street - Cheesecake Rasp White Choc Brulee Sliced</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>Saratoga Sparkling 12oz</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>Smoked Salmon (Retail Pack)</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>Tuna - Ahi (Sesame Seared)</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>Vita Coco - Coconut Water 500ml</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>Vita Coco - Pineapple</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>Grandma's Coffee Cake - Cinnamon</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>Joe Tea - Lemon</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>Java Box (96oz)</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>Java Box (160oz)</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>Monin - Cinnamon</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>Monin - Coconut</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>Tissues/Kleenex</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>Grandma's Coffee Cake - Apple</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>Grandma's Coffee Cake - Blueberry</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>Grandma's Coffee Cake - Chocolate Walnut</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>Iced Tea - Black</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>Copy Paper (8.5" x 11")</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>Mustard - Honey</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>Butter - Salted</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>Nuts - Walnut Halves &amp; Pieces</t>
-        </is>
-      </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>Flour - Millers Choice</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr">
         <is>
           <t>1</t>
         </is>

</xml_diff>